<commit_message>
+ add percent to report
</commit_message>
<xml_diff>
--- a/full_report.xlsx
+++ b/full_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>URL</t>
   </si>
@@ -39,13 +39,16 @@
   </si>
   <si>
     <t>Количество URL</t>
+  </si>
+  <si>
+    <t>Процент</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,6 +64,14 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -70,12 +81,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -84,10 +110,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -382,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -394,26 +420,30 @@
     <col min="2" max="2" width="51.42578125" customWidth="1"/>
     <col min="3" max="3" width="33.7109375" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+    <row r="1" spans="1:5" ht="18.75">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" ht="18.75">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" ht="18.75">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -430,7 +460,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="G2" sqref="A2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -445,34 +475,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" ht="18.75">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
* change report struct
</commit_message>
<xml_diff>
--- a/full_report.xlsx
+++ b/full_report.xlsx
@@ -4,18 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="27660" windowHeight="13170"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="27660" windowHeight="13170" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Итог" sheetId="1" r:id="rId1"/>
     <sheet name="Детальный отчет" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Детальный отчет'!$G$1:$G$2</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>URL</t>
   </si>
@@ -81,7 +84,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -104,16 +107,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -408,47 +423,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="51.42578125" customWidth="1"/>
-    <col min="3" max="3" width="33.7109375" customWidth="1"/>
-    <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="51.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+    <row r="1" spans="1:3" ht="18.75">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:5" ht="18.75">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:3" ht="18.75">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -459,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="A2:G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -475,38 +481,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" ht="18.75">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="G1:G2"/>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>

</xml_diff>

<commit_message>
+new report pages for HTTP and HTTPS
</commit_message>
<xml_diff>
--- a/full_report.xlsx
+++ b/full_report.xlsx
@@ -4,21 +4,23 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="27660" windowHeight="13170" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="27660" windowHeight="13170"/>
   </bookViews>
   <sheets>
     <sheet name="Итог" sheetId="1" r:id="rId1"/>
-    <sheet name="Детальный отчет" sheetId="2" r:id="rId2"/>
+    <sheet name="Итог HTTP" sheetId="3" r:id="rId2"/>
+    <sheet name="Итог HTTPS" sheetId="4" r:id="rId3"/>
+    <sheet name="Детальный отчет" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Детальный отчет'!$G$1:$G$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Детальный отчет'!$G$1:$G$2</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>URL</t>
   </si>
@@ -123,10 +125,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -425,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -437,9 +439,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" ht="18.75">
       <c r="A2" s="1" t="s">
@@ -463,9 +465,87 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="51.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" ht="18.75">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="51.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" ht="18.75">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -481,13 +561,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="18.75">
       <c r="A2" s="1" t="s">

</xml_diff>